<commit_message>
feat(units): add Major Core section to available units panel
- Backend (get_available_units): return unassigned major core units separately
- Frontend (displayAvailableUnits): introduce 'MAJOR CORE' section for drag & drop
- UI now distinguishes between Major Core, Major Electives, and General Electives
</commit_message>
<xml_diff>
--- a/Reference_Material/Essential_Data/Sequence export (MJD-ECNPF).xlsx
+++ b/Reference_Material/Essential_Data/Sequence export (MJD-ECNPF).xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_8F9F684FA3812FF9FA33F31812BE9F0CE70DD7DF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/24409105_student_uwa_edu_au/Documents/UWA/4th semester/cits5206 capstone/AI-Study-Planner-Group8/Reference_Material/Essential_Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_8F9F684FA3812FF9FA33F31812BE9F0CE70DD7DF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A5F9F3E-46B8-425E-817C-A174E8D313FF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2235" yWindow="4980" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequence export" sheetId="1" r:id="rId1"/>
@@ -79,21 +84,6 @@
     <t>Semester 1 2025, Crawley (Face to face); Semester 1 2025, Albany (Face to face); Semester 2 2025, Crawley (Face to face);</t>
   </si>
   <si>
-    <t xml:space="preserve">CB006 Bachelor of Engineering (Honours)/ Bachelor of Commerce as core [Active]; 
-CB017 Bachelor of Philosophy, Politics and Economics and Bachelor of Commerce as core [Active]; 
-CB023 Bachelor of Human Rights and Bachelor of Commerce as core [Active]; 
-CB027 Bachelor of Modern Languages and Bachelor of Commerce as core [Active]; 
-CB048 Bachelor of Media and Communication and Bachelor of Commerce as core [Active]; 
-MJD-ECNSM Business Economics (BCom|*|) as core [Active]; 
-MJD-ECNPF Economics (BEc|*|BEc - MEc|*|) as core [Active]; 
-MJD-PPECN Philosophy, Politics and Economics (BA|*|) as core [Active]; 
-MJD-PPEDM Philosophy, Politics and Economics (BPPE|*|) as core [Active]; 
-MJD-FINEC Financial Economics (BEc|*|) as core [Active]; 
-BP002 Bachelor of Commerce () as core [Active]; 
-BW002 Bachelor of Commerce (Professional) () as core [Proposed]; 
-</t>
-  </si>
-  <si>
     <t>Nil.</t>
   </si>
   <si>
@@ -452,13 +442,6 @@
     <t>History of Economic Ideas</t>
   </si>
   <si>
-    <t xml:space="preserve">MJD-ECNSM Business Economics (BCom|*|) as option [Active]; 
-MJD-ECNPF Economics (BEc|*|BEc - MEc|*|) as option [Active]; 
-MJD-PPECN Philosophy, Politics and Economics (BA|*|) as complementary [Active]; 
-MJD-PPEDM Philosophy, Politics and Economics (BPPE|*|) as option [Active]; 
-</t>
-  </si>
-  <si>
     <t>ECON2233 Microeconomics: Policy and Applications; for pre-2012 courses: none</t>
   </si>
   <si>
@@ -632,12 +615,36 @@
   <si>
     <t>Students are able to (1) apply theoretical concepts to real-life economic issues [assessed by: group project, reflective journal]; (2) analyse appropriate economic  and social data [assessed by: group project, reflective journal]; (3) design an economic report on a specific economic issue. [assessed by: group project]; (4) demonstrate skills in teamwork and problem solving in real world scenarios [assessed by: group project, reflective journal, participation]; (5) demonstrate effective oral and written communication skills [assessed by: group project, reflective journal, participation]; and (6) reflect on performance feedback to identify and action learning opportunities and feedback [assessed by: reflective journal].</t>
   </si>
+  <si>
+    <t xml:space="preserve">CB006 Bachelor of Engineering (Honours)/ Bachelor of Commerce as core [Active]; 
+CB017 Bachelor of Philosophy, Politics and Economics and Bachelor of Commerce as core [Active]; 
+CB023 Bachelor of Human Rights and Bachelor of Commerce as core [Active]; 
+CB027 Bachelor of Modern Languages and Bachelor of Commerce as core [Active]; 
+CB048 Bachelor of Media and Communication and Bachelor of Commerce as core [Active]; 
+MJD-ECNSM Business Economics (BCom|*|) as core [Active]; 
+MJD-ECNPF Economics (BEc|*|BEc - MEc|*|) as core [Active]; 
+MJD-PPECN Philosophy, Politics and Economics (BA|*|) as core [Active]; 
+MJD-PPEDM Philosophy, Politics and Economics (BPPE|*|) as core [Active]; 
+MJD-FINEC Financial Economics (BEc|*|) as core [Active]; 
+BP002 Bachelor of Commerce () as core [Active]; 
+BW002 Bachelor of Commerce (Professional) () as core [Proposed]; 
+</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">MJD-ECNSM Business Economics (BCom|*|) as option [Active]; 
+MJD-ECNPF Economics (BEc|*|BEc - MEc|*|) as option [Active]; 
+MJD-PPECN Philosophy, Politics and Economics (BA|*|) as complementary [Active]; 
+MJD-PPEDM Philosophy, Politics and Economics (BPPE|*|) as option [Active]; 
+</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -648,12 +655,26 @@
       <sz val="17"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="4">
@@ -700,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -714,9 +735,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -1018,14 +1042,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
@@ -1035,7 +1058,7 @@
     <col min="8" max="9" width="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1048,7 +1071,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1061,7 +1084,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1090,7 +1113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>186</v>
       </c>
@@ -1103,779 +1126,780 @@
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
+      <c r="E4" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>187</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:9" ht="285" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>397</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>536</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>215</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1540</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>217</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>495</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>5467</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>8369</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>192</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>206</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+    </row>
+    <row r="16" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>207</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+    </row>
+    <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>7746</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>212</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+    </row>
+    <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>326</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+    </row>
+    <row r="20" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>328</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+    </row>
+    <row r="21" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>208</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="G21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+    </row>
+    <row r="22" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>209</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="G22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+    </row>
+    <row r="23" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>224</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="G23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+    </row>
+    <row r="24" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>231</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="2" t="s">
+      <c r="G24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+    </row>
+    <row r="25" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>232</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="2" t="s">
+      <c r="G25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+    </row>
+    <row r="26" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>241</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="2" t="s">
+      <c r="G26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+    </row>
+    <row r="27" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>5477</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+    </row>
+    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>59</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+    </row>
+    <row r="29" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>7325</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="G29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+    </row>
+    <row r="30" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>7727</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="H30" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A3:I30" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.3543307086614173" right="0.3543307086614173" top="0.3543307086614173" bottom="0.3543307086614173" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape"/>
   <headerFooter>
@@ -1885,18 +1909,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2038,13 +2062,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D74FB7EE-A4AB-4CC6-AFB0-337B2E54C507}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F04EE25-BC4A-4950-BBED-542E4C9D3A07}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F04EE25-BC4A-4950-BBED-542E4C9D3A07}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D74FB7EE-A4AB-4CC6-AFB0-337B2E54C507}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1D84C7F-A279-49F0-8D09-6637CB4FC055}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1D84C7F-A279-49F0-8D09-6637CB4FC055}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f5437da9-3489-479d-94d5-fe8d702a56ae"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>